<commit_message>
Prøvde å legge inn incetive based DR
</commit_message>
<xml_diff>
--- a/Base_Case_Results.xlsx
+++ b/Base_Case_Results.xlsx
@@ -559,7 +559,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>52.20833333333333</v>
+        <v>52.20833333333334</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -4777,7 +4777,7 @@
         <v>0</v>
       </c>
       <c r="K115">
-        <v>65.24958333333333</v>
+        <v>0</v>
       </c>
       <c r="L115">
         <v>0</v>
@@ -10971,7 +10971,7 @@
         <v>0</v>
       </c>
       <c r="K278">
-        <v>43.71666666666667</v>
+        <v>43.71666666666668</v>
       </c>
       <c r="L278">
         <v>0</v>
@@ -12187,7 +12187,7 @@
         <v>0</v>
       </c>
       <c r="K310">
-        <v>51.05833333333333</v>
+        <v>51.05833333333335</v>
       </c>
       <c r="L310">
         <v>0</v>
@@ -15721,7 +15721,7 @@
         <v>0</v>
       </c>
       <c r="K403">
-        <v>79.95</v>
+        <v>79.95000000000002</v>
       </c>
       <c r="L403">
         <v>0</v>
@@ -18077,7 +18077,7 @@
         <v>0</v>
       </c>
       <c r="K465">
-        <v>35.9</v>
+        <v>35.90000000000001</v>
       </c>
       <c r="L465">
         <v>0</v>
@@ -21839,7 +21839,7 @@
         <v>0</v>
       </c>
       <c r="K564">
-        <v>35.45833333333333</v>
+        <v>35.45833333333334</v>
       </c>
       <c r="L564">
         <v>0</v>
@@ -26741,7 +26741,7 @@
         <v>0</v>
       </c>
       <c r="K693">
-        <v>59.25833333333333</v>
+        <v>59.25833333333334</v>
       </c>
       <c r="L693">
         <v>0</v>

</xml_diff>